<commit_message>
Updated transformations, added search strategies, implemented heuristics, added some data files and some general improvements.
</commit_message>
<xml_diff>
--- a/data/icecream.xlsx
+++ b/data/icecream.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gust/mount/home/synthasizer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustv\Projects\synthasizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F8770-36AA-CB48-853A-99AEA2E874E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFF5740-5E93-4A2F-A154-B76474986F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="28280" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icecream" sheetId="1" r:id="rId1"/>
+    <sheet name="header" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
   <si>
     <t>Type</t>
   </si>
@@ -938,13 +939,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -990,7 +991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>18</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1177,7 +1178,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1199,4 +1200,230 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC9112-A996-4D99-93DF-1D0108CED83C}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>170</v>
+      </c>
+      <c r="D3">
+        <v>690</v>
+      </c>
+      <c r="E3">
+        <v>520</v>
+      </c>
+      <c r="F3">
+        <v>1380</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>610</v>
+      </c>
+      <c r="D4">
+        <v>640</v>
+      </c>
+      <c r="E4">
+        <v>320</v>
+      </c>
+      <c r="F4">
+        <v>1570</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>650</v>
+      </c>
+      <c r="E5">
+        <v>630</v>
+      </c>
+      <c r="F5">
+        <v>1530</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>560</v>
+      </c>
+      <c r="D6">
+        <v>320</v>
+      </c>
+      <c r="E6">
+        <v>140</v>
+      </c>
+      <c r="F6">
+        <v>1020</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>430</v>
+      </c>
+      <c r="D7">
+        <v>350</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <v>1080</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>210</v>
+      </c>
+      <c r="D9">
+        <v>280</v>
+      </c>
+      <c r="E9">
+        <v>270</v>
+      </c>
+      <c r="F9">
+        <v>760</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>300</v>
+      </c>
+      <c r="D10">
+        <v>270</v>
+      </c>
+      <c r="E10">
+        <v>290</v>
+      </c>
+      <c r="F10">
+        <v>860</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>610</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>670</v>
+      </c>
+      <c r="F11">
+        <v>1470</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working version on nurse. Relatively fast.
</commit_message>
<xml_diff>
--- a/data/icecream.xlsx
+++ b/data/icecream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustv\Projects\synthasizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFF5740-5E93-4A2F-A154-B76474986F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF94C55-CA18-424C-BB62-090012412066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1692" yWindow="1128" windowWidth="27648" windowHeight="14640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icecream" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1207,219 +1209,233 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>170</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>690</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>520</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>1380</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>610</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>640</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>320</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1570</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>250</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>650</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>630</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>1530</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>560</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>320</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>140</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>1020</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>430</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>350</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>300</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1080</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>210</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>280</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>270</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>760</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>300</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>270</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>290</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>860</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>610</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>190</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>670</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>1470</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>